<commit_message>
updated with performance measures
</commit_message>
<xml_diff>
--- a/dataset_RAG/gemini_rag_results.xlsx
+++ b/dataset_RAG/gemini_rag_results.xlsx
@@ -696,10 +696,8 @@
       <c r="D10" t="n">
         <v>7</v>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>6.5</t>
-        </is>
+      <c r="E10" t="n">
+        <v>6.5</v>
       </c>
       <c r="F10" t="n">
         <v>1.076923076923077</v>
@@ -753,10 +751,8 @@
       <c r="D12" t="n">
         <v>5.5</v>
       </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>6.5</t>
-        </is>
+      <c r="E12" t="n">
+        <v>6.5</v>
       </c>
       <c r="F12" t="n">
         <v>0.8461538461538461</v>
@@ -1632,10 +1628,8 @@
       <c r="D44" t="n">
         <v>6</v>
       </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>5.5</t>
-        </is>
+      <c r="E44" t="n">
+        <v>5.5</v>
       </c>
       <c r="F44" t="n">
         <v>1.090909090909091</v>

</xml_diff>